<commit_message>
add task concept solution X-Life
</commit_message>
<xml_diff>
--- a/WIP/Plans/X-Life_Proposal.xlsx
+++ b/WIP/Plans/X-Life_Proposal.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="184">
   <si>
     <t>Status</t>
   </si>
@@ -577,6 +577,19 @@
   </si>
   <si>
     <t>3/28/2016: đã gởi chi tiết kích thước show-room</t>
+  </si>
+  <si>
+    <t>Xây dựng concept giải pháp X-Life</t>
+  </si>
+  <si>
+    <t>Tìm source code map với demo Arduino Smart Home</t>
+  </si>
+  <si>
+    <t>Tìm demo và source code cho việc hợp nhất các remote</t>
+  </si>
+  <si>
+    <t>Arduino Smart Home Automation: https://www.youtube.com/watch?v=1TF1s9ziu-I
+Arduino Home Security System: https://www.youtube.com/watch?v=dRCnccv_dVE</t>
   </si>
 </sst>
 </file>
@@ -591,7 +604,7 @@
     <numFmt numFmtId="166" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -685,6 +698,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -967,7 +987,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1099,36 +1119,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1148,17 +1138,50 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1171,382 +1194,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -2064,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2084,16 +1732,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -2110,14 +1758,14 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -2197,11 +1845,11 @@
       <c r="C5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
       <c r="G5" s="23" t="s">
         <v>13</v>
       </c>
@@ -2287,20 +1935,20 @@
       <c r="V7" s="7"/>
     </row>
     <row r="8" spans="1:22" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="70">
         <v>42455</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="32" t="s">
         <v>23</v>
       </c>
@@ -2331,20 +1979,20 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="70">
         <v>42455</v>
       </c>
-      <c r="D9" s="89" t="s">
+      <c r="D9" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="89"/>
-      <c r="F9" s="88"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="32" t="s">
         <v>67</v>
       </c>
@@ -2371,20 +2019,20 @@
       <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="80">
+      <c r="C10" s="70">
         <v>42462</v>
       </c>
-      <c r="D10" s="89" t="s">
+      <c r="D10" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="89"/>
-      <c r="F10" s="88"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="77"/>
       <c r="G10" s="32" t="s">
         <v>22</v>
       </c>
@@ -2416,20 +2064,20 @@
       <c r="V10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="80">
+      <c r="C11" s="70">
         <v>42462</v>
       </c>
-      <c r="D11" s="89" t="s">
+      <c r="D11" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="89"/>
-      <c r="F11" s="88"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="32" t="s">
         <v>27</v>
       </c>
@@ -2454,20 +2102,20 @@
       <c r="V11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="70">
         <v>42455</v>
       </c>
-      <c r="D12" s="89" t="s">
+      <c r="D12" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="89"/>
-      <c r="F12" s="88"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="32" t="s">
         <v>27</v>
       </c>
@@ -2492,20 +2140,20 @@
       <c r="V12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="80">
+      <c r="C13" s="70">
         <v>42476</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="89"/>
-      <c r="F13" s="88"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="77"/>
       <c r="G13" s="32" t="s">
         <v>31</v>
       </c>
@@ -2535,21 +2183,21 @@
       <c r="V13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="80">
+      <c r="C14" s="70">
         <f>MAX(C15:C17)</f>
         <v>42476</v>
       </c>
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="88"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="77"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
       <c r="I14" s="33"/>
@@ -2568,20 +2216,20 @@
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="82" t="s">
+      <c r="A15" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="80">
+      <c r="C15" s="70">
         <v>42462</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89" t="s">
+      <c r="D15" s="78"/>
+      <c r="E15" s="78" t="s">
         <v>177</v>
       </c>
-      <c r="F15" s="88"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="32" t="s">
         <v>28</v>
       </c>
@@ -2608,20 +2256,20 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="80">
+      <c r="C16" s="70">
         <v>42462</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89" t="s">
+      <c r="D16" s="78"/>
+      <c r="E16" s="78" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="88"/>
+      <c r="F16" s="77"/>
       <c r="G16" s="32" t="s">
         <v>28</v>
       </c>
@@ -2644,20 +2292,20 @@
       <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="80">
+      <c r="C17" s="70">
         <v>42476</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89" t="s">
+      <c r="D17" s="78"/>
+      <c r="E17" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="88"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="32" t="s">
         <v>22</v>
       </c>
@@ -2682,20 +2330,20 @@
       <c r="V17" s="7"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="82" t="s">
+      <c r="A18" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="80">
+      <c r="C18" s="70">
         <v>42476</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="D18" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="89"/>
-      <c r="F18" s="88"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="77"/>
       <c r="G18" s="32" t="s">
         <v>22</v>
       </c>
@@ -2723,20 +2371,20 @@
       <c r="V18" s="7"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="80">
+      <c r="C19" s="70">
         <v>42476</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="88"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="77"/>
       <c r="G19" s="32" t="s">
         <v>67</v>
       </c>
@@ -2764,21 +2412,21 @@
       <c r="V19" s="7"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="82" t="s">
+      <c r="A20" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="84" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="80">
+      <c r="B20" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="70">
         <f>MAX(C21:C22)</f>
         <v>42476</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="D20" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="E20" s="89"/>
-      <c r="F20" s="87"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="76"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="2"/>
@@ -2799,20 +2447,20 @@
       <c r="V20" s="7"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="80">
+      <c r="C21" s="70">
         <v>42476</v>
       </c>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89" t="s">
+      <c r="D21" s="78"/>
+      <c r="E21" s="78" t="s">
         <v>173</v>
       </c>
-      <c r="F21" s="87"/>
+      <c r="F21" s="76"/>
       <c r="G21" s="1" t="s">
         <v>28</v>
       </c>
@@ -2835,20 +2483,20 @@
       <c r="V21" s="7"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="80">
+      <c r="C22" s="70">
         <v>42476</v>
       </c>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89" t="s">
+      <c r="D22" s="78"/>
+      <c r="E22" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="F22" s="87"/>
+      <c r="F22" s="76"/>
       <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2871,17 +2519,27 @@
       <c r="V22" s="7"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="82"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="87"/>
+      <c r="A23" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="70">
+        <v>42490</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="78"/>
+      <c r="F23" s="76"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="2"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="36"/>
+      <c r="K23" s="36">
+        <v>0</v>
+      </c>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="7"/>
@@ -2894,16 +2552,28 @@
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
-      <c r="B24" s="85"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="1"/>
+    <row r="24" spans="1:22" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="70">
+        <v>42490</v>
+      </c>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24" s="76"/>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="2"/>
+      <c r="I24" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="K24" s="36"/>
       <c r="L24" s="5"/>
@@ -2919,13 +2589,23 @@
       <c r="V24" s="7"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="82"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="70">
+        <v>42490</v>
+      </c>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="F25" s="76"/>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="2"/>
       <c r="J25" s="4"/>
@@ -2943,12 +2623,12 @@
       <c r="V25" s="7"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="82"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="87"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="76"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="2"/>
@@ -2967,12 +2647,12 @@
       <c r="V26" s="7"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="82"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="87"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="76"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="2"/>
@@ -2991,12 +2671,12 @@
       <c r="V27" s="7"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="87"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="76"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="2"/>
@@ -3015,12 +2695,12 @@
       <c r="V28" s="7"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="87"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="76"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="2"/>
@@ -3284,12 +2964,12 @@
         <v>14</v>
       </c>
       <c r="G39" s="27"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="70"/>
-      <c r="K39" s="70"/>
-      <c r="L39" s="70"/>
-      <c r="M39" s="70"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
@@ -3518,12 +3198,12 @@
         <v>14</v>
       </c>
       <c r="G48" s="27"/>
-      <c r="H48" s="69"/>
-      <c r="I48" s="70"/>
-      <c r="J48" s="70"/>
-      <c r="K48" s="70"/>
-      <c r="L48" s="70"/>
-      <c r="M48" s="70"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="80"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="80"/>
+      <c r="M48" s="80"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
@@ -3926,13 +3606,13 @@
     <mergeCell ref="D5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:M365 D21:M21 A8:M19 A20:A21 C20:M20">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>AND($A8="Doing")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="14" stopIfTrue="1">
       <formula>AND($A8="Cancel")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
       <formula>AND($A8="Done")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4455,7 +4135,7 @@
       <c r="D2" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="79" t="s">
+      <c r="E2" s="69" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4674,12 +4354,12 @@
       <c r="C15" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="86"/>
       <c r="H15" s="59"/>
       <c r="I15" s="60"/>
     </row>
@@ -4767,13 +4447,13 @@
       <c r="B19" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
     </row>
@@ -4781,13 +4461,13 @@
       <c r="B20" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="H20" s="55"/>
       <c r="I20" s="55"/>
     </row>
@@ -4803,13 +4483,13 @@
       <c r="B23" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="H23" s="51">
         <v>10</v>
       </c>
@@ -4900,25 +4580,25 @@
       <c r="B28" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C31" s="51" t="s">
@@ -4973,13 +4653,13 @@
       <c r="B33" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">

</xml_diff>

<commit_message>
update plan status, add sample nghien cuu thiet bi
</commit_message>
<xml_diff>
--- a/WIP/Plans/X-Life_Proposal.xlsx
+++ b/WIP/Plans/X-Life_Proposal.xlsx
@@ -14,7 +14,7 @@
     <sheet name="JoinStock" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project Tracking'!$A$3:$V$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Project Tracking'!$B$3:$W$3</definedName>
     <definedName name="priorities">OFFSET(#REF!,1,0,MATCH(REPT("z",255),#REF!),1)</definedName>
     <definedName name="status">OFFSET(#REF!,1,0,MATCH(REPT("z",255),#REF!),1)</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="191">
   <si>
     <t>Status</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Training thi công</t>
-  </si>
-  <si>
-    <t>Thiết kế + thi công showroom</t>
   </si>
   <si>
     <t>BKAV + HaiPM</t>
@@ -615,6 +612,19 @@
 - Khả năng lập trình được
 - Khả năng điều khiển cơ động (ví dụ camera có thẻ xoay tối đa bao nhiêu độ, điều khiển được từ xa hay không)
 - Tương thích với chuẩn IoT nào?</t>
+  </si>
+  <si>
+    <t>Thiết kế showroom</t>
+  </si>
+  <si>
+    <t>Thi công show room</t>
+  </si>
+  <si>
+    <t>1. Kiếm nhà thầu và thương thảo giá cả việc thi công thạch cao trần + đèn + cửa kính
+2. Mapping với thiết kế từ BKAV chốt giá và thực hiện</t>
+  </si>
+  <si>
+    <t>Idx</t>
   </si>
 </sst>
 </file>
@@ -788,7 +798,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1038,6 +1048,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="55"/>
+      </left>
+      <right style="thin">
+        <color indexed="55"/>
+      </right>
+      <top style="thin">
+        <color indexed="55"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="55"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1049,7 +1087,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1107,9 +1145,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1201,6 +1236,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1225,21 +1275,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -1621,68 +1684,68 @@
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="59" t="s">
-        <v>153</v>
+      <c r="B1" s="58" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1692,47 +1755,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="3.625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="40.625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17.875" style="26" customWidth="1"/>
-    <col min="9" max="9" width="20.875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="11" style="7"/>
-    <col min="11" max="11" width="14.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="7"/>
+    <col min="1" max="1" width="3.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="40.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="17.875" style="26" customWidth="1"/>
+    <col min="10" max="10" width="30.875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="11" style="7"/>
+    <col min="12" max="12" width="14.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84">
+    <row r="1" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75">
         <f ca="1">TODAY()</f>
-        <v>42458</v>
-      </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="6"/>
+        <v>42459</v>
+      </c>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -1746,28 +1809,28 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
-    </row>
-    <row r="2" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13"/>
+      <c r="L2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="6"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1776,44 +1839,47 @@
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="E3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="L3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="M3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="N3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1822,27 +1888,27 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40">
-        <f>SUM(K5:K26)</f>
+      <c r="F4" s="77"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="39">
+        <f>SUM(L5:L27)</f>
         <v>350344000</v>
       </c>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="6"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -1851,42 +1917,45 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
-    </row>
-    <row r="5" spans="1:22" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="68" t="s">
+      <c r="W4" s="6"/>
+    </row>
+    <row r="5" spans="1:23" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="32">
+        <v>1</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="65">
+      <c r="D5" s="64">
         <v>42455</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="E5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="I5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="J5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="4">
         <v>1</v>
       </c>
-      <c r="K5" s="31">
+      <c r="L5" s="30">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>8</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1895,38 +1964,41 @@
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
-    </row>
-    <row r="6" spans="1:22" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" s="68" t="s">
+      <c r="W5" s="6"/>
+    </row>
+    <row r="6" spans="1:23" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="32">
+        <v>2</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="65">
+      <c r="D6" s="64">
         <v>42455</v>
       </c>
-      <c r="D6" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="73"/>
+      <c r="E6" s="72" t="s">
+        <v>73</v>
+      </c>
       <c r="F6" s="72"/>
-      <c r="G6" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="G6" s="71"/>
+      <c r="H6" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="K6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="31">
+      <c r="L6" s="30">
         <v>0</v>
       </c>
-      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1935,43 +2007,46 @@
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
-    </row>
-    <row r="7" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="68" t="s">
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="32">
+        <v>3</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="65">
+      <c r="D7" s="64">
         <v>42462</v>
       </c>
-      <c r="D7" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="72" t="s">
+        <v>58</v>
+      </c>
       <c r="F7" s="72"/>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="71"/>
+      <c r="H7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="I7" s="27"/>
+      <c r="J7" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" s="4">
         <v>1</v>
       </c>
-      <c r="K7" s="31">
+      <c r="L7" s="30">
         <f>Budget!E8</f>
         <v>90000000</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>20</v>
       </c>
-      <c r="M7" s="5">
+      <c r="N7" s="5">
         <v>30</v>
       </c>
-      <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1980,38 +2055,41 @@
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A8" s="67" t="s">
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="32">
+        <v>4</v>
+      </c>
+      <c r="B8" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="C8" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="65">
+      <c r="D8" s="64">
         <v>42462</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="E8" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="73"/>
       <c r="F8" s="72"/>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="71"/>
+      <c r="H8" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="I8" s="27"/>
+      <c r="J8" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="K8" s="4">
         <v>0.2</v>
       </c>
-      <c r="K8" s="31">
+      <c r="L8" s="30">
         <v>2000000</v>
       </c>
-      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
+      <c r="N8" s="5"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -2020,38 +2098,41 @@
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" s="69" t="s">
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="32">
+        <v>5</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="65">
+      <c r="D9" s="64">
         <v>42455</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="E9" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="73"/>
       <c r="F9" s="72"/>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="71"/>
+      <c r="H9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="4">
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="4">
         <v>1</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="5">
-        <v>8</v>
-      </c>
+      <c r="L9" s="30"/>
       <c r="M9" s="5">
         <v>8</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="N9" s="5">
+        <v>8</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -2060,41 +2141,44 @@
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A10" s="67" t="s">
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="32">
+        <v>6</v>
+      </c>
+      <c r="B10" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="C10" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="65">
+      <c r="D10" s="64">
         <v>42476</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="E10" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="72"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="I10" s="27"/>
+      <c r="J10" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="31">
+      <c r="L10" s="30">
         <f>Budget!E3</f>
         <v>169344000</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>40</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -2103,31 +2187,39 @@
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="65">
-        <f>MAX(C12:C14)</f>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" ht="45" x14ac:dyDescent="0.2">
+      <c r="A11" s="32">
+        <v>7</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="89">
         <v>42476</v>
       </c>
-      <c r="D11" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
+      <c r="E11" s="90" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="90"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92" t="s">
+        <v>189</v>
+      </c>
+      <c r="K11" s="93">
+        <v>0</v>
+      </c>
+      <c r="L11" s="94"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="95"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -2136,38 +2228,36 @@
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A12" s="67" t="s">
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="32">
+        <v>8</v>
+      </c>
+      <c r="B12" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="C12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="65">
-        <v>42462</v>
-      </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73" t="s">
-        <v>175</v>
+      <c r="D12" s="64">
+        <f>MAX(D13:D15)</f>
+        <v>42476</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>172</v>
       </c>
       <c r="F12" s="72"/>
-      <c r="G12" s="27" t="s">
-        <v>26</v>
-      </c>
+      <c r="G12" s="71"/>
       <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="4">
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="4">
         <v>0</v>
       </c>
-      <c r="K12" s="31">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <v>20</v>
-      </c>
+      <c r="L12" s="30"/>
       <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
+      <c r="N12" s="5"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -2176,34 +2266,41 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A13" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="69" t="s">
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="32">
+        <v>9</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="65">
+      <c r="D13" s="64">
         <v>42462</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="72"/>
+      <c r="F13" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="72"/>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="71"/>
+      <c r="H13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="31">
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="4">
         <v>0</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
+      <c r="L13" s="30">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>20</v>
+      </c>
+      <c r="N13" s="5"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -2212,36 +2309,37 @@
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A14" s="67" t="s">
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="32">
+        <v>10</v>
+      </c>
+      <c r="B14" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="C14" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="65">
-        <v>42476</v>
-      </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="31">
-        <v>5000000</v>
-      </c>
-      <c r="L14" s="5">
-        <v>40</v>
+      <c r="D14" s="64">
+        <v>42462</v>
+      </c>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72" t="s">
+        <v>173</v>
+      </c>
+      <c r="G14" s="71"/>
+      <c r="H14" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="30">
+        <v>0</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="6"/>
+      <c r="N14" s="5"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -2250,39 +2348,39 @@
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A15" s="67" t="s">
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="32">
+        <v>11</v>
+      </c>
+      <c r="B15" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="C15" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="65">
+      <c r="D15" s="64">
         <v>42476</v>
       </c>
-      <c r="D15" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="73"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="27" t="s">
+      <c r="E15" s="72"/>
+      <c r="F15" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="71"/>
+      <c r="H15" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="31">
-        <f>Budget!E10</f>
-        <v>48000000</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="30">
+        <v>5000000</v>
+      </c>
+      <c r="M15" s="5">
         <v>40</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6"/>
+      <c r="N15" s="5"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -2291,39 +2389,42 @@
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A16" s="67" t="s">
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="32">
+        <v>12</v>
+      </c>
+      <c r="B16" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="69" t="s">
+      <c r="C16" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="65">
+      <c r="D16" s="64">
         <v>42476</v>
       </c>
-      <c r="D16" s="73" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="73"/>
+      <c r="E16" s="72" t="s">
+        <v>27</v>
+      </c>
       <c r="F16" s="72"/>
-      <c r="G16" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="31">
-        <f>Budget!E9</f>
-        <v>36000000</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="G16" s="71"/>
+      <c r="H16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="30">
+        <f>Budget!E10</f>
+        <v>48000000</v>
+      </c>
+      <c r="M16" s="5">
         <v>40</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="6"/>
+      <c r="N16" s="5"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -2332,33 +2433,42 @@
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="67" t="s">
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="32">
+        <v>13</v>
+      </c>
+      <c r="B17" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="65">
-        <f>MAX(C18:C19)</f>
+      <c r="C17" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="64">
         <v>42476</v>
       </c>
-      <c r="D17" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="E17" s="73"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="31">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
+      <c r="E17" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="72"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="30">
+        <f>Budget!E9</f>
+        <v>36000000</v>
+      </c>
+      <c r="M17" s="5">
+        <v>40</v>
+      </c>
+      <c r="N17" s="5"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
@@ -2367,36 +2477,36 @@
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
-    </row>
-    <row r="18" spans="1:22" ht="112.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="68" t="s">
+      <c r="W17" s="6"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="32">
+        <v>14</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="65">
+      <c r="D18" s="64">
+        <f>MAX(D19:D20)</f>
         <v>42476</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="F18" s="71"/>
-      <c r="G18" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E18" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="31">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="30">
         <v>0</v>
       </c>
-      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
-      <c r="N18" s="6"/>
+      <c r="N18" s="5"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
@@ -2405,36 +2515,39 @@
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
-    </row>
-    <row r="19" spans="1:22" ht="135" x14ac:dyDescent="0.2">
-      <c r="A19" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="68" t="s">
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" ht="90" x14ac:dyDescent="0.2">
+      <c r="A19" s="32">
+        <v>15</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="65">
+      <c r="D19" s="64">
         <v>42476</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19" s="71"/>
-      <c r="G19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1" t="s">
+      <c r="E19" s="72"/>
+      <c r="F19" s="72" t="s">
+        <v>170</v>
+      </c>
+      <c r="G19" s="70"/>
+      <c r="H19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="31">
+      <c r="K19" s="4"/>
+      <c r="L19" s="30">
         <v>0</v>
       </c>
-      <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="6"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -2443,32 +2556,39 @@
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="67" t="s">
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" ht="112.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="32">
+        <v>16</v>
+      </c>
+      <c r="B20" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="65">
-        <v>42490</v>
-      </c>
-      <c r="D20" s="73" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="73"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="31">
+      <c r="C20" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="64">
+        <v>42476</v>
+      </c>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="G20" s="70"/>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="30">
         <v>0</v>
       </c>
-      <c r="L20" s="5"/>
       <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -2477,34 +2597,35 @@
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
-    </row>
-    <row r="21" spans="1:22" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="67" t="s">
+      <c r="W20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="32">
         <v>17</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="65">
+      <c r="D21" s="64">
         <v>42490</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73" t="s">
-        <v>179</v>
-      </c>
-      <c r="F21" s="71"/>
-      <c r="G21" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="E21" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="72"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="5"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="30">
+        <v>0</v>
+      </c>
       <c r="M21" s="5"/>
-      <c r="N21" s="6"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -2513,32 +2634,37 @@
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="67" t="s">
+      <c r="W21" s="6"/>
+    </row>
+    <row r="22" spans="1:23" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="32">
+        <v>18</v>
+      </c>
+      <c r="B22" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="65">
+      <c r="D22" s="64">
         <v>42490</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73" t="s">
+      <c r="E22" s="72"/>
+      <c r="F22" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="70"/>
+      <c r="H22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="30"/>
       <c r="M22" s="5"/>
-      <c r="N22" s="6"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
@@ -2547,22 +2673,35 @@
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="67"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="5"/>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="32">
+        <v>19</v>
+      </c>
+      <c r="B23" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="64">
+        <v>42490</v>
+      </c>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="H23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="30"/>
       <c r="M23" s="5"/>
-      <c r="N23" s="6"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
@@ -2571,22 +2710,22 @@
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="67"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="1"/>
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B24" s="66"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="70"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="5"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="30"/>
       <c r="M24" s="5"/>
-      <c r="N24" s="6"/>
+      <c r="N24" s="5"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -2595,22 +2734,22 @@
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="67"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="1"/>
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B25" s="66"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="5"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="30"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="6"/>
+      <c r="N25" s="5"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
@@ -2619,24 +2758,22 @@
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="67"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="1"/>
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B26" s="66"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="70"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="31">
-        <v>0</v>
-      </c>
-      <c r="L26" s="5"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="30"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="6"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
@@ -2645,24 +2782,24 @@
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="6"/>
+      <c r="W26" s="6"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B27" s="66"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="30">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -2671,24 +2808,24 @@
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="6"/>
+      <c r="W27" s="6"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="24"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -2697,24 +2834,24 @@
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="W28" s="6"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B29" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="5"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="30"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="6"/>
+      <c r="N29" s="5"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="6"/>
@@ -2723,24 +2860,24 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="W29" s="6"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B30" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="5"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="30"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="6"/>
+      <c r="N30" s="5"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
@@ -2749,24 +2886,24 @@
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
       <c r="V30" s="6"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="W30" s="6"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B31" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="5"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="30"/>
       <c r="M31" s="5"/>
-      <c r="N31" s="6"/>
+      <c r="N31" s="5"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -2775,24 +2912,24 @@
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
       <c r="V31" s="6"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="W31" s="6"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B32" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="5"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="30"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="6"/>
+      <c r="N32" s="5"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
@@ -2801,24 +2938,24 @@
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
       <c r="V32" s="6"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="W32" s="6"/>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B33" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="1"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="5"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="30"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
@@ -2827,24 +2964,24 @@
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
       <c r="V33" s="6"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="W33" s="6"/>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B34" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="5"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="30"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="6"/>
+      <c r="N34" s="5"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
@@ -2853,24 +2990,24 @@
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
       <c r="V34" s="6"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="W34" s="6"/>
+    </row>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B35" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="5"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="30"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="6"/>
+      <c r="N35" s="5"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
@@ -2879,9 +3016,24 @@
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N36" s="6"/>
+      <c r="W35" s="6"/>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B36" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
@@ -2890,9 +3042,9 @@
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N37" s="6"/>
+      <c r="W36" s="6"/>
+    </row>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="6"/>
@@ -2901,9 +3053,9 @@
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N38" s="6"/>
+      <c r="W37" s="6"/>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
@@ -2912,9 +3064,9 @@
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
       <c r="V38" s="6"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N39" s="6"/>
+      <c r="W38" s="6"/>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
@@ -2923,9 +3075,9 @@
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
       <c r="V39" s="6"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N40" s="6"/>
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="6"/>
@@ -2934,9 +3086,9 @@
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
       <c r="V40" s="6"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N41" s="6"/>
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="6"/>
@@ -2945,9 +3097,9 @@
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
       <c r="V41" s="6"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N42" s="6"/>
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
@@ -2956,9 +3108,9 @@
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
       <c r="V42" s="6"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N43" s="6"/>
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
@@ -2967,9 +3119,9 @@
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
       <c r="V43" s="6"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N44" s="6"/>
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
@@ -2978,9 +3130,9 @@
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N45" s="6"/>
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
@@ -2989,9 +3141,9 @@
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N46" s="6"/>
+      <c r="W45" s="6"/>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
@@ -3000,9 +3152,9 @@
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N47" s="6"/>
+      <c r="W46" s="6"/>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="6"/>
@@ -3011,9 +3163,9 @@
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
       <c r="V47" s="6"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N48" s="6"/>
+      <c r="W47" s="6"/>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="6"/>
@@ -3022,9 +3174,9 @@
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
-    </row>
-    <row r="49" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N49" s="6"/>
+      <c r="W48" s="6"/>
+    </row>
+    <row r="49" spans="15:23" x14ac:dyDescent="0.2">
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
@@ -3033,9 +3185,9 @@
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
       <c r="V49" s="6"/>
-    </row>
-    <row r="50" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N50" s="6"/>
+      <c r="W49" s="6"/>
+    </row>
+    <row r="50" spans="15:23" x14ac:dyDescent="0.2">
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
       <c r="Q50" s="6"/>
@@ -3044,9 +3196,9 @@
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
-    </row>
-    <row r="51" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N51" s="6"/>
+      <c r="W50" s="6"/>
+    </row>
+    <row r="51" spans="15:23" x14ac:dyDescent="0.2">
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
@@ -3055,31 +3207,43 @@
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
       <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+    </row>
+    <row r="52" spans="15:23" x14ac:dyDescent="0.2">
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:V3">
+  <autoFilter ref="B3:W3">
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="E3:G3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D18:M18 A5:M16 A17:A18 C17:M17 A26:M344">
+  <conditionalFormatting sqref="E19:N19 B5:N17 B18:B19 D18:N18 B27:N345">
     <cfRule type="expression" dxfId="2" priority="13" stopIfTrue="1">
-      <formula>AND($A5="Doing")</formula>
+      <formula>AND($B5="Doing")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="14" stopIfTrue="1">
-      <formula>AND($A5="Cancel")</formula>
+      <formula>AND($B5="Cancel")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="15" stopIfTrue="1">
-      <formula>AND($A5="Done")</formula>
+      <formula>AND($B5="Done")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A28:A35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29:B36">
       <formula1>"NotStart,Doing,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B27">
       <formula1>"NotStart,Doing,Done,Cancel"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3113,440 +3277,440 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="32">
+        <v>57</v>
+      </c>
+      <c r="E2" s="31">
         <f>E8</f>
         <v>90000000</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="31">
         <f>E2/12</f>
         <v>7500000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="32">
+        <v>56</v>
+      </c>
+      <c r="E3" s="31">
         <f>SUM(E11:E23)</f>
         <v>169344000</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="41">
         <f>E3/36</f>
         <v>4704000</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="32">
+        <v>67</v>
+      </c>
+      <c r="E4" s="31">
         <f>SUM(E9:E10)</f>
         <v>84000000</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <f>E4/12</f>
         <v>7000000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32">
+        <v>70</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31">
         <f>SUM(F2:F4)</f>
         <v>19204000</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D6" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32">
+      <c r="D6" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31">
         <f>F5*5</f>
         <v>96020000</v>
       </c>
-      <c r="G6" s="41" t="s">
-        <v>73</v>
+      <c r="G6" s="40" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="34" t="s">
+      <c r="A7" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="D7" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="F7" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="G7" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>1</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
-        <v>1</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35">
         <f>F8*12</f>
         <v>90000000</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>7500000</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>37</v>
+      <c r="G8" s="36" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>2</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36">
+      <c r="B9" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="35">
         <f>F9*12</f>
         <v>36000000</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="35">
         <v>3000000</v>
       </c>
-      <c r="G9" s="37" t="s">
-        <v>63</v>
+      <c r="G9" s="36" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
+      <c r="A10" s="34">
         <v>3</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36">
+      <c r="B10" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35">
         <f>F10*12</f>
         <v>48000000</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="35">
         <v>4000000</v>
       </c>
-      <c r="G10" s="37" t="s">
-        <v>63</v>
+      <c r="G10" s="36" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+      <c r="A11" s="34">
         <v>4</v>
       </c>
-      <c r="B11" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36">
+      <c r="B11" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35">
         <f>SUM(F12:F24)*1.1</f>
         <v>157344000</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="35" t="s">
-        <v>64</v>
+      <c r="F11" s="35"/>
+      <c r="G11" s="34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="34">
         <v>5</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35">
+        <v>6000000</v>
+      </c>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>6</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36">
-        <v>6000000</v>
-      </c>
-      <c r="G12" s="35"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
-        <v>6</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35" t="s">
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35">
+        <v>4000000</v>
+      </c>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>7</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36">
-        <v>4000000</v>
-      </c>
-      <c r="G13" s="35"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
-        <v>7</v>
-      </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35" t="s">
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35">
+        <v>15000000</v>
+      </c>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
+        <v>8</v>
+      </c>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36">
-        <v>15000000</v>
-      </c>
-      <c r="G14" s="35"/>
-    </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
-        <v>8</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35" t="s">
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35">
+        <v>0</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
+        <v>9</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
+        <v>1800000</v>
+      </c>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
+        <v>10</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36">
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35">
+        <v>5000000</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
+        <v>11</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35">
         <v>0</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G18" s="36" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
-        <v>9</v>
-      </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
+        <v>12</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36">
-        <v>1800000</v>
-      </c>
-      <c r="G16" s="35"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
-        <v>10</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36">
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35">
         <v>5000000</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G19" s="34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <v>13</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35">
+        <v>1000000</v>
+      </c>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
+        <v>14</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35">
+        <v>5000000</v>
+      </c>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="34">
+        <v>15</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
-        <v>11</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36">
-        <v>0</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="35">
-        <v>12</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36">
-        <v>5000000</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
-        <v>13</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36">
-        <v>1000000</v>
-      </c>
-      <c r="G20" s="35"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
-        <v>14</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36">
-        <v>5000000</v>
-      </c>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
-        <v>15</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35">
         <f>F22*40</f>
         <v>4800000</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="35">
         <v>120000</v>
       </c>
-      <c r="G22" s="35" t="s">
-        <v>54</v>
+      <c r="G22" s="34" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="35">
+      <c r="A23" s="34">
         <v>16</v>
       </c>
-      <c r="B23" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36">
+      <c r="B23" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35">
         <f>F23*60</f>
         <v>7200000</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="35">
         <v>120000</v>
       </c>
-      <c r="G23" s="35" t="s">
-        <v>55</v>
+      <c r="G23" s="34" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
+      <c r="A24" s="34">
         <v>17</v>
       </c>
-      <c r="B24" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36">
+      <c r="B24" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35">
         <v>100000000</v>
       </c>
-      <c r="G24" s="35"/>
+      <c r="G24" s="34"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="35"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="34"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="35"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="34"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="35"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="35"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
@@ -3571,11 +3735,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3585,119 +3747,155 @@
     <col min="4" max="4" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" s="63" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="44" t="s">
+      <c r="C3" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="64" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="96">
         <v>42452</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-    </row>
-    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-    </row>
-    <row r="8" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="47" t="s">
+      <c r="B9" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46" t="s">
+      <c r="C9" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="D9" s="45"/>
+      <c r="E9" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="45"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="96">
+        <v>42452</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46" t="s">
+      <c r="C10" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46" t="s">
+      <c r="D10" s="45"/>
+      <c r="E10" s="45" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>42452</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3724,21 +3922,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>121</v>
+      <c r="A2" s="58" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
-        <v>134</v>
+      <c r="B3" s="58" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3746,12 +3944,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3759,17 +3957,17 @@
         <v>1.2</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3777,7 +3975,7 @@
         <v>1.3</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3785,356 +3983,356 @@
         <v>1.4</v>
       </c>
       <c r="C11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="59" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="60" t="s">
+      <c r="D12" t="s">
         <v>131</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="59" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="60" t="s">
-        <v>133</v>
-      </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.5</v>
       </c>
-      <c r="C14" s="62" t="s">
-        <v>120</v>
+      <c r="C14" s="61" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="45"/>
+      <c r="C15" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="55"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="C16" s="46" t="s">
+      <c r="D16" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="46">
+      <c r="C17" s="45">
         <v>4</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="45">
         <v>4</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="45">
         <v>4</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="45">
         <v>4</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="45">
         <v>4</v>
       </c>
-      <c r="H17" s="46">
+      <c r="H17" s="45">
         <f>SUM(C17:G17)</f>
         <v>20</v>
       </c>
-      <c r="I17" s="61">
+      <c r="I17" s="60">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="61">
+      <c r="B18" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="60">
         <f>$I$17*C17/$H$17</f>
         <v>0.04</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="60">
         <f>$I$17*D17/$H$17</f>
         <v>0.04</v>
       </c>
-      <c r="E18" s="61">
+      <c r="E18" s="60">
         <f>$I$17*E17/$H$17</f>
         <v>0.04</v>
       </c>
-      <c r="F18" s="61">
+      <c r="F18" s="60">
         <f>$I$17*F17/$H$17</f>
         <v>0.04</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="60">
         <f>$I$17*G17/$H$17</f>
         <v>0.04</v>
       </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="52"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="58" t="s">
+      <c r="B19" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="80" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="80" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>101</v>
+      <c r="H22" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80"/>
-      <c r="H23" s="46">
+      <c r="B23" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="45">
         <v>10</v>
       </c>
-      <c r="I23" s="61">
+      <c r="I23" s="60">
         <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="I25" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="56">
+      <c r="C26" s="55">
         <v>100000000</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="55">
         <v>50000000</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="55">
         <v>50000000</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F26" s="55">
         <v>50000000</v>
       </c>
-      <c r="G26" s="56">
+      <c r="G26" s="55">
         <v>0</v>
       </c>
-      <c r="H26" s="57">
+      <c r="H26" s="56">
         <f>SUM(C26:G26)</f>
         <v>250000000</v>
       </c>
-      <c r="I26" s="61">
+      <c r="I26" s="60">
         <f>100%-I23-I17</f>
         <v>0.7</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="61">
+      <c r="B27" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="60">
         <f>$I$26*(C26/$H$26)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="60">
         <f>$I$26*(D26/$H$26)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E27" s="61">
+      <c r="E27" s="60">
         <f>$I$26*(E26/$H$26)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F27" s="61">
+      <c r="F27" s="60">
         <f>$I$26*(F26/$H$26)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G27" s="61">
+      <c r="G27" s="60">
         <f>$I$26*(G26/$H$26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="82" t="s">
+      <c r="B28" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="86" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="82"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C31" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="H31" s="53" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="61">
+      <c r="C32" s="60">
         <f>C18+C27</f>
         <v>0.31999999999999995</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="60">
         <f t="shared" ref="D32:F32" si="0">D18+D27</f>
         <v>0.18</v>
       </c>
-      <c r="E32" s="61">
+      <c r="E32" s="60">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="F32" s="61">
+      <c r="F32" s="60">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="G32" s="61">
+      <c r="G32" s="60">
         <f>G18+G27+I23</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="H32" s="49">
+      <c r="H32" s="48">
         <f>SUM(C32:G32)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
+      <c r="B33" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
-      <c r="B35" s="59" t="s">
-        <v>135</v>
+      <c r="B35" s="58" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -4142,7 +4340,7 @@
         <v>2.1</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -4150,15 +4348,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
-      <c r="B39" s="59" t="s">
-        <v>92</v>
+      <c r="B39" s="58" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -4166,7 +4364,7 @@
         <v>2.1</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -4174,7 +4372,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -4182,20 +4380,20 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
-      <c r="B43" s="59" t="s">
-        <v>140</v>
+      <c r="B43" s="58" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -4203,7 +4401,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -4211,7 +4409,7 @@
         <v>4.2</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -4219,15 +4417,15 @@
         <v>4.3</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
-      <c r="B48" s="59" t="s">
-        <v>141</v>
+      <c r="B48" s="58" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4235,55 +4433,55 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="62">
+      <c r="B50" s="61">
         <v>5.2</v>
       </c>
       <c r="C50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="61">
+        <v>5.3</v>
+      </c>
+      <c r="C51" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="62">
-        <v>5.3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>143</v>
-      </c>
-    </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="62">
+      <c r="B52" s="61">
         <v>5.4</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
-      <c r="B53" s="59" t="s">
-        <v>95</v>
+      <c r="B53" s="58" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="62">
+      <c r="B54" s="61">
         <v>6.1</v>
       </c>
       <c r="C54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="61">
+        <v>6.2</v>
+      </c>
+      <c r="C55" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="62">
-        <v>6.2</v>
-      </c>
-      <c r="C55" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mẫu phòng khách, mô hình giải pháp smart home
</commit_message>
<xml_diff>
--- a/WIP/Plans/X-Life_Proposal.xlsx
+++ b/WIP/Plans/X-Life_Proposal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37800" yWindow="-2145" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-37800" yWindow="-2145" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Proposal" sheetId="5" r:id="rId1"/>
@@ -1097,7 +1097,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1312,6 +1312,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1767,11 +1772,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1802,7 +1807,7 @@
       <c r="F1" s="74"/>
       <c r="G1" s="75">
         <f ca="1">TODAY()</f>
-        <v>42462</v>
+        <v>42463</v>
       </c>
       <c r="H1" s="74"/>
       <c r="I1" s="74"/>
@@ -3271,8 +3276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3503,19 +3508,19 @@
       <c r="G14" s="34"/>
     </row>
     <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="97">
         <v>8</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34" t="s">
+      <c r="B15" s="97"/>
+      <c r="C15" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35">
+      <c r="D15" s="97"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98">
         <v>0</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="99" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3552,19 +3557,19 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+      <c r="A18" s="97">
         <v>11</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34" t="s">
+      <c r="B18" s="97"/>
+      <c r="C18" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35">
+      <c r="D18" s="97"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98">
         <v>0</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="99" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>